<commit_message>
Updated with back button
</commit_message>
<xml_diff>
--- a/education/cadw_bp/dialogue/npc.xlsx
+++ b/education/cadw_bp/dialogue/npc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK110"/>
+  <dimension ref="A1:AR110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,27 +596,62 @@
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
+          <t>Button Name Welsh 2</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Button Name Welsh 3</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
           <t>Button Name 2</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Button Name 3</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Button Name 4</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Button Name Welsh 4</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Command Button Welsh 4</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Button Name 5</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Button Name Welsh 5</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Command Button Welsh 5</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Button Name 6</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Button Name Welsh 6</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Command Button Welsh 6</t>
         </is>
       </c>
     </row>
@@ -662,6 +697,13 @@
       <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -705,6 +747,13 @@
       <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -808,6 +857,13 @@
       <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -879,6 +935,13 @@
       <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -974,6 +1037,13 @@
       <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1069,6 +1139,13 @@
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1164,6 +1241,13 @@
       <c r="AI8" t="inlineStr"/>
       <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1259,6 +1343,13 @@
       <c r="AI9" t="inlineStr"/>
       <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1354,6 +1445,13 @@
       <c r="AI10" t="inlineStr"/>
       <c r="AJ10" t="inlineStr"/>
       <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1449,6 +1547,13 @@
       <c r="AI11" t="inlineStr"/>
       <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1544,6 +1649,13 @@
       <c r="AI12" t="inlineStr"/>
       <c r="AJ12" t="inlineStr"/>
       <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
+      <c r="AR12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1639,6 +1751,13 @@
       <c r="AI13" t="inlineStr"/>
       <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1735,6 +1854,13 @@
       <c r="AI14" t="inlineStr"/>
       <c r="AJ14" t="inlineStr"/>
       <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1830,6 +1956,13 @@
       <c r="AI15" t="inlineStr"/>
       <c r="AJ15" t="inlineStr"/>
       <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1909,6 +2042,13 @@
       <c r="AI16" t="inlineStr"/>
       <c r="AJ16" t="inlineStr"/>
       <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1988,6 +2128,13 @@
       <c r="AI17" t="inlineStr"/>
       <c r="AJ17" t="inlineStr"/>
       <c r="AK17" t="inlineStr"/>
+      <c r="AL17" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr"/>
+      <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
+      <c r="AR17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2083,6 +2230,13 @@
       <c r="AI18" t="inlineStr"/>
       <c r="AJ18" t="inlineStr"/>
       <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="inlineStr"/>
+      <c r="AQ18" t="inlineStr"/>
+      <c r="AR18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2178,6 +2332,13 @@
       <c r="AI19" t="inlineStr"/>
       <c r="AJ19" t="inlineStr"/>
       <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
+      <c r="AR19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2273,6 +2434,13 @@
       <c r="AI20" t="inlineStr"/>
       <c r="AJ20" t="inlineStr"/>
       <c r="AK20" t="inlineStr"/>
+      <c r="AL20" t="inlineStr"/>
+      <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="inlineStr"/>
+      <c r="AQ20" t="inlineStr"/>
+      <c r="AR20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2368,6 +2536,13 @@
       <c r="AI21" t="inlineStr"/>
       <c r="AJ21" t="inlineStr"/>
       <c r="AK21" t="inlineStr"/>
+      <c r="AL21" t="inlineStr"/>
+      <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr"/>
+      <c r="AO21" t="inlineStr"/>
+      <c r="AP21" t="inlineStr"/>
+      <c r="AQ21" t="inlineStr"/>
+      <c r="AR21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2463,6 +2638,13 @@
       <c r="AI22" t="inlineStr"/>
       <c r="AJ22" t="inlineStr"/>
       <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="inlineStr"/>
+      <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr"/>
+      <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="inlineStr"/>
+      <c r="AQ22" t="inlineStr"/>
+      <c r="AR22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2558,6 +2740,13 @@
       <c r="AI23" t="inlineStr"/>
       <c r="AJ23" t="inlineStr"/>
       <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr"/>
+      <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr"/>
+      <c r="AO23" t="inlineStr"/>
+      <c r="AP23" t="inlineStr"/>
+      <c r="AQ23" t="inlineStr"/>
+      <c r="AR23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2653,6 +2842,13 @@
       <c r="AI24" t="inlineStr"/>
       <c r="AJ24" t="inlineStr"/>
       <c r="AK24" t="inlineStr"/>
+      <c r="AL24" t="inlineStr"/>
+      <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr"/>
+      <c r="AO24" t="inlineStr"/>
+      <c r="AP24" t="inlineStr"/>
+      <c r="AQ24" t="inlineStr"/>
+      <c r="AR24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2748,6 +2944,13 @@
       <c r="AI25" t="inlineStr"/>
       <c r="AJ25" t="inlineStr"/>
       <c r="AK25" t="inlineStr"/>
+      <c r="AL25" t="inlineStr"/>
+      <c r="AM25" t="inlineStr"/>
+      <c r="AN25" t="inlineStr"/>
+      <c r="AO25" t="inlineStr"/>
+      <c r="AP25" t="inlineStr"/>
+      <c r="AQ25" t="inlineStr"/>
+      <c r="AR25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2843,6 +3046,13 @@
       <c r="AI26" t="inlineStr"/>
       <c r="AJ26" t="inlineStr"/>
       <c r="AK26" t="inlineStr"/>
+      <c r="AL26" t="inlineStr"/>
+      <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="inlineStr"/>
+      <c r="AO26" t="inlineStr"/>
+      <c r="AP26" t="inlineStr"/>
+      <c r="AQ26" t="inlineStr"/>
+      <c r="AR26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2922,6 +3132,13 @@
       <c r="AI27" t="inlineStr"/>
       <c r="AJ27" t="inlineStr"/>
       <c r="AK27" t="inlineStr"/>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr"/>
+      <c r="AO27" t="inlineStr"/>
+      <c r="AP27" t="inlineStr"/>
+      <c r="AQ27" t="inlineStr"/>
+      <c r="AR27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3017,6 +3234,13 @@
       <c r="AI28" t="inlineStr"/>
       <c r="AJ28" t="inlineStr"/>
       <c r="AK28" t="inlineStr"/>
+      <c r="AL28" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
+      <c r="AP28" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
+      <c r="AR28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3112,6 +3336,13 @@
       <c r="AI29" t="inlineStr"/>
       <c r="AJ29" t="inlineStr"/>
       <c r="AK29" t="inlineStr"/>
+      <c r="AL29" t="inlineStr"/>
+      <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr"/>
+      <c r="AO29" t="inlineStr"/>
+      <c r="AP29" t="inlineStr"/>
+      <c r="AQ29" t="inlineStr"/>
+      <c r="AR29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3239,6 +3470,13 @@
       <c r="AI30" t="inlineStr"/>
       <c r="AJ30" t="inlineStr"/>
       <c r="AK30" t="inlineStr"/>
+      <c r="AL30" t="inlineStr"/>
+      <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr"/>
+      <c r="AO30" t="inlineStr"/>
+      <c r="AP30" t="inlineStr"/>
+      <c r="AQ30" t="inlineStr"/>
+      <c r="AR30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3354,6 +3592,13 @@
       <c r="AI31" t="inlineStr"/>
       <c r="AJ31" t="inlineStr"/>
       <c r="AK31" t="inlineStr"/>
+      <c r="AL31" t="inlineStr"/>
+      <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr"/>
+      <c r="AO31" t="inlineStr"/>
+      <c r="AP31" t="inlineStr"/>
+      <c r="AQ31" t="inlineStr"/>
+      <c r="AR31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3513,6 +3758,13 @@
       <c r="AI32" t="inlineStr"/>
       <c r="AJ32" t="inlineStr"/>
       <c r="AK32" t="inlineStr"/>
+      <c r="AL32" t="inlineStr"/>
+      <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr"/>
+      <c r="AO32" t="inlineStr"/>
+      <c r="AP32" t="inlineStr"/>
+      <c r="AQ32" t="inlineStr"/>
+      <c r="AR32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3624,6 +3876,13 @@
       <c r="AI33" t="inlineStr"/>
       <c r="AJ33" t="inlineStr"/>
       <c r="AK33" t="inlineStr"/>
+      <c r="AL33" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr"/>
+      <c r="AO33" t="inlineStr"/>
+      <c r="AP33" t="inlineStr"/>
+      <c r="AQ33" t="inlineStr"/>
+      <c r="AR33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3735,6 +3994,13 @@
       <c r="AI34" t="inlineStr"/>
       <c r="AJ34" t="inlineStr"/>
       <c r="AK34" t="inlineStr"/>
+      <c r="AL34" t="inlineStr"/>
+      <c r="AM34" t="inlineStr"/>
+      <c r="AN34" t="inlineStr"/>
+      <c r="AO34" t="inlineStr"/>
+      <c r="AP34" t="inlineStr"/>
+      <c r="AQ34" t="inlineStr"/>
+      <c r="AR34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3846,6 +4112,13 @@
       <c r="AI35" t="inlineStr"/>
       <c r="AJ35" t="inlineStr"/>
       <c r="AK35" t="inlineStr"/>
+      <c r="AL35" t="inlineStr"/>
+      <c r="AM35" t="inlineStr"/>
+      <c r="AN35" t="inlineStr"/>
+      <c r="AO35" t="inlineStr"/>
+      <c r="AP35" t="inlineStr"/>
+      <c r="AQ35" t="inlineStr"/>
+      <c r="AR35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3957,6 +4230,13 @@
       <c r="AI36" t="inlineStr"/>
       <c r="AJ36" t="inlineStr"/>
       <c r="AK36" t="inlineStr"/>
+      <c r="AL36" t="inlineStr"/>
+      <c r="AM36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr"/>
+      <c r="AO36" t="inlineStr"/>
+      <c r="AP36" t="inlineStr"/>
+      <c r="AQ36" t="inlineStr"/>
+      <c r="AR36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4068,6 +4348,13 @@
       <c r="AI37" t="inlineStr"/>
       <c r="AJ37" t="inlineStr"/>
       <c r="AK37" t="inlineStr"/>
+      <c r="AL37" t="inlineStr"/>
+      <c r="AM37" t="inlineStr"/>
+      <c r="AN37" t="inlineStr"/>
+      <c r="AO37" t="inlineStr"/>
+      <c r="AP37" t="inlineStr"/>
+      <c r="AQ37" t="inlineStr"/>
+      <c r="AR37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4179,6 +4466,13 @@
       <c r="AI38" t="inlineStr"/>
       <c r="AJ38" t="inlineStr"/>
       <c r="AK38" t="inlineStr"/>
+      <c r="AL38" t="inlineStr"/>
+      <c r="AM38" t="inlineStr"/>
+      <c r="AN38" t="inlineStr"/>
+      <c r="AO38" t="inlineStr"/>
+      <c r="AP38" t="inlineStr"/>
+      <c r="AQ38" t="inlineStr"/>
+      <c r="AR38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4222,6 +4516,13 @@
       <c r="AI39" t="inlineStr"/>
       <c r="AJ39" t="inlineStr"/>
       <c r="AK39" t="inlineStr"/>
+      <c r="AL39" t="inlineStr"/>
+      <c r="AM39" t="inlineStr"/>
+      <c r="AN39" t="inlineStr"/>
+      <c r="AO39" t="inlineStr"/>
+      <c r="AP39" t="inlineStr"/>
+      <c r="AQ39" t="inlineStr"/>
+      <c r="AR39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4293,6 +4594,13 @@
       <c r="AI40" t="inlineStr"/>
       <c r="AJ40" t="inlineStr"/>
       <c r="AK40" t="inlineStr"/>
+      <c r="AL40" t="inlineStr"/>
+      <c r="AM40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr"/>
+      <c r="AO40" t="inlineStr"/>
+      <c r="AP40" t="inlineStr"/>
+      <c r="AQ40" t="inlineStr"/>
+      <c r="AR40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4452,6 +4760,13 @@
       <c r="AI41" t="inlineStr"/>
       <c r="AJ41" t="inlineStr"/>
       <c r="AK41" t="inlineStr"/>
+      <c r="AL41" t="inlineStr"/>
+      <c r="AM41" t="inlineStr"/>
+      <c r="AN41" t="inlineStr"/>
+      <c r="AO41" t="inlineStr"/>
+      <c r="AP41" t="inlineStr"/>
+      <c r="AQ41" t="inlineStr"/>
+      <c r="AR41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4523,6 +4838,13 @@
       <c r="AI42" t="inlineStr"/>
       <c r="AJ42" t="inlineStr"/>
       <c r="AK42" t="inlineStr"/>
+      <c r="AL42" t="inlineStr"/>
+      <c r="AM42" t="inlineStr"/>
+      <c r="AN42" t="inlineStr"/>
+      <c r="AO42" t="inlineStr"/>
+      <c r="AP42" t="inlineStr"/>
+      <c r="AQ42" t="inlineStr"/>
+      <c r="AR42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4634,6 +4956,13 @@
       <c r="AI43" t="inlineStr"/>
       <c r="AJ43" t="inlineStr"/>
       <c r="AK43" t="inlineStr"/>
+      <c r="AL43" t="inlineStr"/>
+      <c r="AM43" t="inlineStr"/>
+      <c r="AN43" t="inlineStr"/>
+      <c r="AO43" t="inlineStr"/>
+      <c r="AP43" t="inlineStr"/>
+      <c r="AQ43" t="inlineStr"/>
+      <c r="AR43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4729,6 +5058,13 @@
       <c r="AI44" t="inlineStr"/>
       <c r="AJ44" t="inlineStr"/>
       <c r="AK44" t="inlineStr"/>
+      <c r="AL44" t="inlineStr"/>
+      <c r="AM44" t="inlineStr"/>
+      <c r="AN44" t="inlineStr"/>
+      <c r="AO44" t="inlineStr"/>
+      <c r="AP44" t="inlineStr"/>
+      <c r="AQ44" t="inlineStr"/>
+      <c r="AR44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4800,6 +5136,13 @@
       <c r="AI45" t="inlineStr"/>
       <c r="AJ45" t="inlineStr"/>
       <c r="AK45" t="inlineStr"/>
+      <c r="AL45" t="inlineStr"/>
+      <c r="AM45" t="inlineStr"/>
+      <c r="AN45" t="inlineStr"/>
+      <c r="AO45" t="inlineStr"/>
+      <c r="AP45" t="inlineStr"/>
+      <c r="AQ45" t="inlineStr"/>
+      <c r="AR45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4887,6 +5230,13 @@
       <c r="AI46" t="inlineStr"/>
       <c r="AJ46" t="inlineStr"/>
       <c r="AK46" t="inlineStr"/>
+      <c r="AL46" t="inlineStr"/>
+      <c r="AM46" t="inlineStr"/>
+      <c r="AN46" t="inlineStr"/>
+      <c r="AO46" t="inlineStr"/>
+      <c r="AP46" t="inlineStr"/>
+      <c r="AQ46" t="inlineStr"/>
+      <c r="AR46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4958,6 +5308,13 @@
       <c r="AI47" t="inlineStr"/>
       <c r="AJ47" t="inlineStr"/>
       <c r="AK47" t="inlineStr"/>
+      <c r="AL47" t="inlineStr"/>
+      <c r="AM47" t="inlineStr"/>
+      <c r="AN47" t="inlineStr"/>
+      <c r="AO47" t="inlineStr"/>
+      <c r="AP47" t="inlineStr"/>
+      <c r="AQ47" t="inlineStr"/>
+      <c r="AR47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5073,6 +5430,13 @@
       <c r="AI48" t="inlineStr"/>
       <c r="AJ48" t="inlineStr"/>
       <c r="AK48" t="inlineStr"/>
+      <c r="AL48" t="inlineStr"/>
+      <c r="AM48" t="inlineStr"/>
+      <c r="AN48" t="inlineStr"/>
+      <c r="AO48" t="inlineStr"/>
+      <c r="AP48" t="inlineStr"/>
+      <c r="AQ48" t="inlineStr"/>
+      <c r="AR48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5200,6 +5564,13 @@
       <c r="AI49" t="inlineStr"/>
       <c r="AJ49" t="inlineStr"/>
       <c r="AK49" t="inlineStr"/>
+      <c r="AL49" t="inlineStr"/>
+      <c r="AM49" t="inlineStr"/>
+      <c r="AN49" t="inlineStr"/>
+      <c r="AO49" t="inlineStr"/>
+      <c r="AP49" t="inlineStr"/>
+      <c r="AQ49" t="inlineStr"/>
+      <c r="AR49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5311,6 +5682,13 @@
       <c r="AI50" t="inlineStr"/>
       <c r="AJ50" t="inlineStr"/>
       <c r="AK50" t="inlineStr"/>
+      <c r="AL50" t="inlineStr"/>
+      <c r="AM50" t="inlineStr"/>
+      <c r="AN50" t="inlineStr"/>
+      <c r="AO50" t="inlineStr"/>
+      <c r="AP50" t="inlineStr"/>
+      <c r="AQ50" t="inlineStr"/>
+      <c r="AR50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5354,6 +5732,13 @@
       <c r="AI51" t="inlineStr"/>
       <c r="AJ51" t="inlineStr"/>
       <c r="AK51" t="inlineStr"/>
+      <c r="AL51" t="inlineStr"/>
+      <c r="AM51" t="inlineStr"/>
+      <c r="AN51" t="inlineStr"/>
+      <c r="AO51" t="inlineStr"/>
+      <c r="AP51" t="inlineStr"/>
+      <c r="AQ51" t="inlineStr"/>
+      <c r="AR51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5417,6 +5802,13 @@
       <c r="AI52" t="inlineStr"/>
       <c r="AJ52" t="inlineStr"/>
       <c r="AK52" t="inlineStr"/>
+      <c r="AL52" t="inlineStr"/>
+      <c r="AM52" t="inlineStr"/>
+      <c r="AN52" t="inlineStr"/>
+      <c r="AO52" t="inlineStr"/>
+      <c r="AP52" t="inlineStr"/>
+      <c r="AQ52" t="inlineStr"/>
+      <c r="AR52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5488,6 +5880,13 @@
       <c r="AI53" t="inlineStr"/>
       <c r="AJ53" t="inlineStr"/>
       <c r="AK53" t="inlineStr"/>
+      <c r="AL53" t="inlineStr"/>
+      <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr"/>
+      <c r="AO53" t="inlineStr"/>
+      <c r="AP53" t="inlineStr"/>
+      <c r="AQ53" t="inlineStr"/>
+      <c r="AR53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5567,6 +5966,13 @@
       <c r="AI54" t="inlineStr"/>
       <c r="AJ54" t="inlineStr"/>
       <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr"/>
+      <c r="AO54" t="inlineStr"/>
+      <c r="AP54" t="inlineStr"/>
+      <c r="AQ54" t="inlineStr"/>
+      <c r="AR54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
@@ -5606,6 +6012,13 @@
       <c r="AI55" t="inlineStr"/>
       <c r="AJ55" t="inlineStr"/>
       <c r="AK55" t="inlineStr"/>
+      <c r="AL55" t="inlineStr"/>
+      <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr"/>
+      <c r="AO55" t="inlineStr"/>
+      <c r="AP55" t="inlineStr"/>
+      <c r="AQ55" t="inlineStr"/>
+      <c r="AR55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr"/>
@@ -5645,6 +6058,13 @@
       <c r="AI56" t="inlineStr"/>
       <c r="AJ56" t="inlineStr"/>
       <c r="AK56" t="inlineStr"/>
+      <c r="AL56" t="inlineStr"/>
+      <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr"/>
+      <c r="AO56" t="inlineStr"/>
+      <c r="AP56" t="inlineStr"/>
+      <c r="AQ56" t="inlineStr"/>
+      <c r="AR56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr"/>
@@ -5684,6 +6104,13 @@
       <c r="AI57" t="inlineStr"/>
       <c r="AJ57" t="inlineStr"/>
       <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr"/>
+      <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr"/>
+      <c r="AO57" t="inlineStr"/>
+      <c r="AP57" t="inlineStr"/>
+      <c r="AQ57" t="inlineStr"/>
+      <c r="AR57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr"/>
@@ -5723,6 +6150,13 @@
       <c r="AI58" t="inlineStr"/>
       <c r="AJ58" t="inlineStr"/>
       <c r="AK58" t="inlineStr"/>
+      <c r="AL58" t="inlineStr"/>
+      <c r="AM58" t="inlineStr"/>
+      <c r="AN58" t="inlineStr"/>
+      <c r="AO58" t="inlineStr"/>
+      <c r="AP58" t="inlineStr"/>
+      <c r="AQ58" t="inlineStr"/>
+      <c r="AR58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5766,6 +6200,13 @@
       <c r="AI59" t="inlineStr"/>
       <c r="AJ59" t="inlineStr"/>
       <c r="AK59" t="inlineStr"/>
+      <c r="AL59" t="inlineStr"/>
+      <c r="AM59" t="inlineStr"/>
+      <c r="AN59" t="inlineStr"/>
+      <c r="AO59" t="inlineStr"/>
+      <c r="AP59" t="inlineStr"/>
+      <c r="AQ59" t="inlineStr"/>
+      <c r="AR59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5876,6 +6317,13 @@
       <c r="AI60" t="inlineStr"/>
       <c r="AJ60" t="inlineStr"/>
       <c r="AK60" t="inlineStr"/>
+      <c r="AL60" t="inlineStr"/>
+      <c r="AM60" t="inlineStr"/>
+      <c r="AN60" t="inlineStr"/>
+      <c r="AO60" t="inlineStr"/>
+      <c r="AP60" t="inlineStr"/>
+      <c r="AQ60" t="inlineStr"/>
+      <c r="AR60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5920,8 +6368,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=8YTWeHO-Wa8 </t>
         </is>
       </c>
-      <c r="K61" t="inlineStr"/>
-      <c r="L61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinNPC] taliesinNPC1</t>
+        </is>
+      </c>
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
@@ -5944,11 +6400,7 @@
         </is>
       </c>
       <c r="V61" t="inlineStr"/>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
       <c r="Z61" t="inlineStr"/>
@@ -5963,10 +6415,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH61" t="inlineStr"/>
-      <c r="AI61" t="inlineStr"/>
+      <c r="AH61" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI61" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ61" t="inlineStr"/>
       <c r="AK61" t="inlineStr"/>
+      <c r="AL61" t="inlineStr"/>
+      <c r="AM61" t="inlineStr"/>
+      <c r="AN61" t="inlineStr"/>
+      <c r="AO61" t="inlineStr"/>
+      <c r="AP61" t="inlineStr"/>
+      <c r="AQ61" t="inlineStr"/>
+      <c r="AR61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6011,8 +6478,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=03QngMoJ3pc </t>
         </is>
       </c>
-      <c r="K62" t="inlineStr"/>
-      <c r="L62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinNPC] taliesinNPC1</t>
+        </is>
+      </c>
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
@@ -6035,11 +6510,7 @@
         </is>
       </c>
       <c r="V62" t="inlineStr"/>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W62" t="inlineStr"/>
       <c r="X62" t="inlineStr"/>
       <c r="Y62" t="inlineStr"/>
       <c r="Z62" t="inlineStr"/>
@@ -6054,10 +6525,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH62" t="inlineStr"/>
-      <c r="AI62" t="inlineStr"/>
+      <c r="AH62" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI62" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ62" t="inlineStr"/>
       <c r="AK62" t="inlineStr"/>
+      <c r="AL62" t="inlineStr"/>
+      <c r="AM62" t="inlineStr"/>
+      <c r="AN62" t="inlineStr"/>
+      <c r="AO62" t="inlineStr"/>
+      <c r="AP62" t="inlineStr"/>
+      <c r="AQ62" t="inlineStr"/>
+      <c r="AR62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6102,8 +6588,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=hmWzvGu3N4A </t>
         </is>
       </c>
-      <c r="K63" t="inlineStr"/>
-      <c r="L63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=pcNPC] pcNPC1</t>
+        </is>
+      </c>
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
@@ -6126,11 +6620,7 @@
         </is>
       </c>
       <c r="V63" t="inlineStr"/>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W63" t="inlineStr"/>
       <c r="X63" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
       <c r="Z63" t="inlineStr"/>
@@ -6145,10 +6635,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH63" t="inlineStr"/>
-      <c r="AI63" t="inlineStr"/>
+      <c r="AH63" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI63" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ63" t="inlineStr"/>
       <c r="AK63" t="inlineStr"/>
+      <c r="AL63" t="inlineStr"/>
+      <c r="AM63" t="inlineStr"/>
+      <c r="AN63" t="inlineStr"/>
+      <c r="AO63" t="inlineStr"/>
+      <c r="AP63" t="inlineStr"/>
+      <c r="AQ63" t="inlineStr"/>
+      <c r="AR63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6193,8 +6698,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=Ck8mqnSioQw </t>
         </is>
       </c>
-      <c r="K64" t="inlineStr"/>
-      <c r="L64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=wbNPC] wbNPC1</t>
+        </is>
+      </c>
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr"/>
@@ -6217,11 +6730,7 @@
         </is>
       </c>
       <c r="V64" t="inlineStr"/>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W64" t="inlineStr"/>
       <c r="X64" t="inlineStr"/>
       <c r="Y64" t="inlineStr"/>
       <c r="Z64" t="inlineStr"/>
@@ -6236,10 +6745,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH64" t="inlineStr"/>
-      <c r="AI64" t="inlineStr"/>
+      <c r="AH64" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI64" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ64" t="inlineStr"/>
       <c r="AK64" t="inlineStr"/>
+      <c r="AL64" t="inlineStr"/>
+      <c r="AM64" t="inlineStr"/>
+      <c r="AN64" t="inlineStr"/>
+      <c r="AO64" t="inlineStr"/>
+      <c r="AP64" t="inlineStr"/>
+      <c r="AQ64" t="inlineStr"/>
+      <c r="AR64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -6284,8 +6808,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=12B2IYOJDnw </t>
         </is>
       </c>
-      <c r="K65" t="inlineStr"/>
-      <c r="L65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=mgNPC] mgNPC1</t>
+        </is>
+      </c>
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
@@ -6308,11 +6840,7 @@
         </is>
       </c>
       <c r="V65" t="inlineStr"/>
-      <c r="W65" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W65" t="inlineStr"/>
       <c r="X65" t="inlineStr"/>
       <c r="Y65" t="inlineStr"/>
       <c r="Z65" t="inlineStr"/>
@@ -6327,10 +6855,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH65" t="inlineStr"/>
-      <c r="AI65" t="inlineStr"/>
+      <c r="AH65" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI65" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ65" t="inlineStr"/>
       <c r="AK65" t="inlineStr"/>
+      <c r="AL65" t="inlineStr"/>
+      <c r="AM65" t="inlineStr"/>
+      <c r="AN65" t="inlineStr"/>
+      <c r="AO65" t="inlineStr"/>
+      <c r="AP65" t="inlineStr"/>
+      <c r="AQ65" t="inlineStr"/>
+      <c r="AR65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6375,8 +6918,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=FGxhtFeKAxA </t>
         </is>
       </c>
-      <c r="K66" t="inlineStr"/>
-      <c r="L66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=owNPC] owNPC1</t>
+        </is>
+      </c>
       <c r="M66" t="inlineStr"/>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
@@ -6399,11 +6950,7 @@
         </is>
       </c>
       <c r="V66" t="inlineStr"/>
-      <c r="W66" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W66" t="inlineStr"/>
       <c r="X66" t="inlineStr"/>
       <c r="Y66" t="inlineStr"/>
       <c r="Z66" t="inlineStr"/>
@@ -6418,10 +6965,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH66" t="inlineStr"/>
-      <c r="AI66" t="inlineStr"/>
+      <c r="AH66" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI66" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ66" t="inlineStr"/>
       <c r="AK66" t="inlineStr"/>
+      <c r="AL66" t="inlineStr"/>
+      <c r="AM66" t="inlineStr"/>
+      <c r="AN66" t="inlineStr"/>
+      <c r="AO66" t="inlineStr"/>
+      <c r="AP66" t="inlineStr"/>
+      <c r="AQ66" t="inlineStr"/>
+      <c r="AR66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6466,8 +7028,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=ltjz9fCDelY </t>
         </is>
       </c>
-      <c r="K67" t="inlineStr"/>
-      <c r="L67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=nwtNPC] nwtNPC1</t>
+        </is>
+      </c>
       <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
@@ -6490,11 +7060,7 @@
         </is>
       </c>
       <c r="V67" t="inlineStr"/>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W67" t="inlineStr"/>
       <c r="X67" t="inlineStr"/>
       <c r="Y67" t="inlineStr"/>
       <c r="Z67" t="inlineStr"/>
@@ -6509,10 +7075,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH67" t="inlineStr"/>
-      <c r="AI67" t="inlineStr"/>
+      <c r="AH67" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI67" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ67" t="inlineStr"/>
       <c r="AK67" t="inlineStr"/>
+      <c r="AL67" t="inlineStr"/>
+      <c r="AM67" t="inlineStr"/>
+      <c r="AN67" t="inlineStr"/>
+      <c r="AO67" t="inlineStr"/>
+      <c r="AP67" t="inlineStr"/>
+      <c r="AQ67" t="inlineStr"/>
+      <c r="AR67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -6557,8 +7138,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=rmOew_MSHo0 </t>
         </is>
       </c>
-      <c r="K68" t="inlineStr"/>
-      <c r="L68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=swtNPC] swtNPC1</t>
+        </is>
+      </c>
       <c r="M68" t="inlineStr"/>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
@@ -6581,11 +7170,7 @@
         </is>
       </c>
       <c r="V68" t="inlineStr"/>
-      <c r="W68" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W68" t="inlineStr"/>
       <c r="X68" t="inlineStr"/>
       <c r="Y68" t="inlineStr"/>
       <c r="Z68" t="inlineStr"/>
@@ -6600,10 +7185,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH68" t="inlineStr"/>
-      <c r="AI68" t="inlineStr"/>
+      <c r="AH68" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI68" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ68" t="inlineStr"/>
       <c r="AK68" t="inlineStr"/>
+      <c r="AL68" t="inlineStr"/>
+      <c r="AM68" t="inlineStr"/>
+      <c r="AN68" t="inlineStr"/>
+      <c r="AO68" t="inlineStr"/>
+      <c r="AP68" t="inlineStr"/>
+      <c r="AQ68" t="inlineStr"/>
+      <c r="AR68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6648,8 +7248,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=JjkXGwGUjnM </t>
         </is>
       </c>
-      <c r="K69" t="inlineStr"/>
-      <c r="L69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=cghNPC] cghNPC1</t>
+        </is>
+      </c>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
@@ -6672,11 +7280,7 @@
         </is>
       </c>
       <c r="V69" t="inlineStr"/>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W69" t="inlineStr"/>
       <c r="X69" t="inlineStr"/>
       <c r="Y69" t="inlineStr"/>
       <c r="Z69" t="inlineStr"/>
@@ -6691,10 +7295,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH69" t="inlineStr"/>
-      <c r="AI69" t="inlineStr"/>
+      <c r="AH69" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI69" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ69" t="inlineStr"/>
       <c r="AK69" t="inlineStr"/>
+      <c r="AL69" t="inlineStr"/>
+      <c r="AM69" t="inlineStr"/>
+      <c r="AN69" t="inlineStr"/>
+      <c r="AO69" t="inlineStr"/>
+      <c r="AP69" t="inlineStr"/>
+      <c r="AQ69" t="inlineStr"/>
+      <c r="AR69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6739,8 +7358,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=Fk4yKbs8bh8 </t>
         </is>
       </c>
-      <c r="K70" t="inlineStr"/>
-      <c r="L70" t="inlineStr"/>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ptNPC] ptNPC1</t>
+        </is>
+      </c>
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
@@ -6763,11 +7390,7 @@
         </is>
       </c>
       <c r="V70" t="inlineStr"/>
-      <c r="W70" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W70" t="inlineStr"/>
       <c r="X70" t="inlineStr"/>
       <c r="Y70" t="inlineStr"/>
       <c r="Z70" t="inlineStr"/>
@@ -6782,10 +7405,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH70" t="inlineStr"/>
-      <c r="AI70" t="inlineStr"/>
+      <c r="AH70" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI70" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ70" t="inlineStr"/>
       <c r="AK70" t="inlineStr"/>
+      <c r="AL70" t="inlineStr"/>
+      <c r="AM70" t="inlineStr"/>
+      <c r="AN70" t="inlineStr"/>
+      <c r="AO70" t="inlineStr"/>
+      <c r="AP70" t="inlineStr"/>
+      <c r="AQ70" t="inlineStr"/>
+      <c r="AR70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -6830,8 +7468,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=EPRkmH1UcRs </t>
         </is>
       </c>
-      <c r="K71" t="inlineStr"/>
-      <c r="L71" t="inlineStr"/>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=kitchNPC] kitchNPC1</t>
+        </is>
+      </c>
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
@@ -6854,11 +7500,7 @@
         </is>
       </c>
       <c r="V71" t="inlineStr"/>
-      <c r="W71" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W71" t="inlineStr"/>
       <c r="X71" t="inlineStr"/>
       <c r="Y71" t="inlineStr"/>
       <c r="Z71" t="inlineStr"/>
@@ -6873,10 +7515,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH71" t="inlineStr"/>
-      <c r="AI71" t="inlineStr"/>
+      <c r="AH71" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI71" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ71" t="inlineStr"/>
       <c r="AK71" t="inlineStr"/>
+      <c r="AL71" t="inlineStr"/>
+      <c r="AM71" t="inlineStr"/>
+      <c r="AN71" t="inlineStr"/>
+      <c r="AO71" t="inlineStr"/>
+      <c r="AP71" t="inlineStr"/>
+      <c r="AQ71" t="inlineStr"/>
+      <c r="AR71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -6921,8 +7578,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=9vw1epEJZfk </t>
         </is>
       </c>
-      <c r="K72" t="inlineStr"/>
-      <c r="L72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=wellNPC] wellNPC1</t>
+        </is>
+      </c>
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
@@ -6945,11 +7610,7 @@
         </is>
       </c>
       <c r="V72" t="inlineStr"/>
-      <c r="W72" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W72" t="inlineStr"/>
       <c r="X72" t="inlineStr"/>
       <c r="Y72" t="inlineStr"/>
       <c r="Z72" t="inlineStr"/>
@@ -6964,10 +7625,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH72" t="inlineStr"/>
-      <c r="AI72" t="inlineStr"/>
+      <c r="AH72" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI72" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ72" t="inlineStr"/>
       <c r="AK72" t="inlineStr"/>
+      <c r="AL72" t="inlineStr"/>
+      <c r="AM72" t="inlineStr"/>
+      <c r="AN72" t="inlineStr"/>
+      <c r="AO72" t="inlineStr"/>
+      <c r="AP72" t="inlineStr"/>
+      <c r="AQ72" t="inlineStr"/>
+      <c r="AR72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7012,8 +7688,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=4VWRwmfvS14 </t>
         </is>
       </c>
-      <c r="K73" t="inlineStr"/>
-      <c r="L73" t="inlineStr"/>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=midgNPC] midgNPC1</t>
+        </is>
+      </c>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
@@ -7036,11 +7720,7 @@
         </is>
       </c>
       <c r="V73" t="inlineStr"/>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W73" t="inlineStr"/>
       <c r="X73" t="inlineStr"/>
       <c r="Y73" t="inlineStr"/>
       <c r="Z73" t="inlineStr"/>
@@ -7055,10 +7735,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH73" t="inlineStr"/>
-      <c r="AI73" t="inlineStr"/>
+      <c r="AH73" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI73" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ73" t="inlineStr"/>
       <c r="AK73" t="inlineStr"/>
+      <c r="AL73" t="inlineStr"/>
+      <c r="AM73" t="inlineStr"/>
+      <c r="AN73" t="inlineStr"/>
+      <c r="AO73" t="inlineStr"/>
+      <c r="AP73" t="inlineStr"/>
+      <c r="AQ73" t="inlineStr"/>
+      <c r="AR73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -7103,8 +7798,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=9Lb2bOrvwQ4 </t>
         </is>
       </c>
-      <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=iwNPC] iwNPC1</t>
+        </is>
+      </c>
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
@@ -7127,11 +7830,7 @@
         </is>
       </c>
       <c r="V74" t="inlineStr"/>
-      <c r="W74" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W74" t="inlineStr"/>
       <c r="X74" t="inlineStr"/>
       <c r="Y74" t="inlineStr"/>
       <c r="Z74" t="inlineStr"/>
@@ -7146,10 +7845,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH74" t="inlineStr"/>
-      <c r="AI74" t="inlineStr"/>
+      <c r="AH74" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI74" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ74" t="inlineStr"/>
       <c r="AK74" t="inlineStr"/>
+      <c r="AL74" t="inlineStr"/>
+      <c r="AM74" t="inlineStr"/>
+      <c r="AN74" t="inlineStr"/>
+      <c r="AO74" t="inlineStr"/>
+      <c r="AP74" t="inlineStr"/>
+      <c r="AQ74" t="inlineStr"/>
+      <c r="AR74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -7194,8 +7908,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=GsX2KAv3n24 </t>
         </is>
       </c>
-      <c r="K75" t="inlineStr"/>
-      <c r="L75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=cgcNPC] cgcNPC1</t>
+        </is>
+      </c>
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr"/>
@@ -7218,11 +7940,7 @@
         </is>
       </c>
       <c r="V75" t="inlineStr"/>
-      <c r="W75" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W75" t="inlineStr"/>
       <c r="X75" t="inlineStr"/>
       <c r="Y75" t="inlineStr"/>
       <c r="Z75" t="inlineStr"/>
@@ -7237,10 +7955,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH75" t="inlineStr"/>
-      <c r="AI75" t="inlineStr"/>
+      <c r="AH75" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI75" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ75" t="inlineStr"/>
       <c r="AK75" t="inlineStr"/>
+      <c r="AL75" t="inlineStr"/>
+      <c r="AM75" t="inlineStr"/>
+      <c r="AN75" t="inlineStr"/>
+      <c r="AO75" t="inlineStr"/>
+      <c r="AP75" t="inlineStr"/>
+      <c r="AQ75" t="inlineStr"/>
+      <c r="AR75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7285,8 +8018,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=BCLEkB_VpoQ </t>
         </is>
       </c>
-      <c r="K76" t="inlineStr"/>
-      <c r="L76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ctNPC] ctNPC1</t>
+        </is>
+      </c>
       <c r="M76" t="inlineStr"/>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
@@ -7309,11 +8050,7 @@
         </is>
       </c>
       <c r="V76" t="inlineStr"/>
-      <c r="W76" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W76" t="inlineStr"/>
       <c r="X76" t="inlineStr"/>
       <c r="Y76" t="inlineStr"/>
       <c r="Z76" t="inlineStr"/>
@@ -7328,10 +8065,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH76" t="inlineStr"/>
-      <c r="AI76" t="inlineStr"/>
+      <c r="AH76" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI76" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ76" t="inlineStr"/>
       <c r="AK76" t="inlineStr"/>
+      <c r="AL76" t="inlineStr"/>
+      <c r="AM76" t="inlineStr"/>
+      <c r="AN76" t="inlineStr"/>
+      <c r="AO76" t="inlineStr"/>
+      <c r="AP76" t="inlineStr"/>
+      <c r="AQ76" t="inlineStr"/>
+      <c r="AR76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -7376,8 +8128,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=so4YnmfCyRM </t>
         </is>
       </c>
-      <c r="K77" t="inlineStr"/>
-      <c r="L77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ctNPC] ctNPC2</t>
+        </is>
+      </c>
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
@@ -7400,11 +8160,7 @@
         </is>
       </c>
       <c r="V77" t="inlineStr"/>
-      <c r="W77" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W77" t="inlineStr"/>
       <c r="X77" t="inlineStr"/>
       <c r="Y77" t="inlineStr"/>
       <c r="Z77" t="inlineStr"/>
@@ -7419,10 +8175,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH77" t="inlineStr"/>
-      <c r="AI77" t="inlineStr"/>
+      <c r="AH77" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI77" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ77" t="inlineStr"/>
       <c r="AK77" t="inlineStr"/>
+      <c r="AL77" t="inlineStr"/>
+      <c r="AM77" t="inlineStr"/>
+      <c r="AN77" t="inlineStr"/>
+      <c r="AO77" t="inlineStr"/>
+      <c r="AP77" t="inlineStr"/>
+      <c r="AQ77" t="inlineStr"/>
+      <c r="AR77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7467,8 +8238,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=V9YfzmsILiQ </t>
         </is>
       </c>
-      <c r="K78" t="inlineStr"/>
-      <c r="L78" t="inlineStr"/>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=wcNPC] wcNPC1</t>
+        </is>
+      </c>
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr"/>
@@ -7491,11 +8270,7 @@
         </is>
       </c>
       <c r="V78" t="inlineStr"/>
-      <c r="W78" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W78" t="inlineStr"/>
       <c r="X78" t="inlineStr"/>
       <c r="Y78" t="inlineStr"/>
       <c r="Z78" t="inlineStr"/>
@@ -7510,10 +8285,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH78" t="inlineStr"/>
-      <c r="AI78" t="inlineStr"/>
+      <c r="AH78" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI78" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ78" t="inlineStr"/>
       <c r="AK78" t="inlineStr"/>
+      <c r="AL78" t="inlineStr"/>
+      <c r="AM78" t="inlineStr"/>
+      <c r="AN78" t="inlineStr"/>
+      <c r="AO78" t="inlineStr"/>
+      <c r="AP78" t="inlineStr"/>
+      <c r="AQ78" t="inlineStr"/>
+      <c r="AR78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7558,8 +8348,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=fNXnaRnsMPs </t>
         </is>
       </c>
-      <c r="K79" t="inlineStr"/>
-      <c r="L79" t="inlineStr"/>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ktNPC] ktNPC1</t>
+        </is>
+      </c>
       <c r="M79" t="inlineStr"/>
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr"/>
@@ -7582,11 +8380,7 @@
         </is>
       </c>
       <c r="V79" t="inlineStr"/>
-      <c r="W79" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W79" t="inlineStr"/>
       <c r="X79" t="inlineStr"/>
       <c r="Y79" t="inlineStr"/>
       <c r="Z79" t="inlineStr"/>
@@ -7601,10 +8395,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH79" t="inlineStr"/>
-      <c r="AI79" t="inlineStr"/>
+      <c r="AH79" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI79" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ79" t="inlineStr"/>
       <c r="AK79" t="inlineStr"/>
+      <c r="AL79" t="inlineStr"/>
+      <c r="AM79" t="inlineStr"/>
+      <c r="AN79" t="inlineStr"/>
+      <c r="AO79" t="inlineStr"/>
+      <c r="AP79" t="inlineStr"/>
+      <c r="AQ79" t="inlineStr"/>
+      <c r="AR79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7649,8 +8458,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=HrCZQz6tZM0 </t>
         </is>
       </c>
-      <c r="K80" t="inlineStr"/>
-      <c r="L80" t="inlineStr"/>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=kcNPC] kcNPC1</t>
+        </is>
+      </c>
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
@@ -7673,11 +8490,7 @@
         </is>
       </c>
       <c r="V80" t="inlineStr"/>
-      <c r="W80" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W80" t="inlineStr"/>
       <c r="X80" t="inlineStr"/>
       <c r="Y80" t="inlineStr"/>
       <c r="Z80" t="inlineStr"/>
@@ -7692,10 +8505,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH80" t="inlineStr"/>
-      <c r="AI80" t="inlineStr"/>
+      <c r="AH80" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI80" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ80" t="inlineStr"/>
       <c r="AK80" t="inlineStr"/>
+      <c r="AL80" t="inlineStr"/>
+      <c r="AM80" t="inlineStr"/>
+      <c r="AN80" t="inlineStr"/>
+      <c r="AO80" t="inlineStr"/>
+      <c r="AP80" t="inlineStr"/>
+      <c r="AQ80" t="inlineStr"/>
+      <c r="AR80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -7740,8 +8568,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=xgritMV1-yc </t>
         </is>
       </c>
-      <c r="K81" t="inlineStr"/>
-      <c r="L81" t="inlineStr"/>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=qcNPC] qcNPC1</t>
+        </is>
+      </c>
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
@@ -7764,11 +8600,7 @@
         </is>
       </c>
       <c r="V81" t="inlineStr"/>
-      <c r="W81" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W81" t="inlineStr"/>
       <c r="X81" t="inlineStr"/>
       <c r="Y81" t="inlineStr"/>
       <c r="Z81" t="inlineStr"/>
@@ -7783,10 +8615,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH81" t="inlineStr"/>
-      <c r="AI81" t="inlineStr"/>
+      <c r="AH81" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI81" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ81" t="inlineStr"/>
       <c r="AK81" t="inlineStr"/>
+      <c r="AL81" t="inlineStr"/>
+      <c r="AM81" t="inlineStr"/>
+      <c r="AN81" t="inlineStr"/>
+      <c r="AO81" t="inlineStr"/>
+      <c r="AP81" t="inlineStr"/>
+      <c r="AQ81" t="inlineStr"/>
+      <c r="AR81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -7831,8 +8678,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=ybA8Uq2faf8 </t>
         </is>
       </c>
-      <c r="K82" t="inlineStr"/>
-      <c r="L82" t="inlineStr"/>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=bhNPC] bhNPC1</t>
+        </is>
+      </c>
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
@@ -7855,11 +8710,7 @@
         </is>
       </c>
       <c r="V82" t="inlineStr"/>
-      <c r="W82" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W82" t="inlineStr"/>
       <c r="X82" t="inlineStr"/>
       <c r="Y82" t="inlineStr"/>
       <c r="Z82" t="inlineStr"/>
@@ -7874,10 +8725,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH82" t="inlineStr"/>
-      <c r="AI82" t="inlineStr"/>
+      <c r="AH82" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI82" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ82" t="inlineStr"/>
       <c r="AK82" t="inlineStr"/>
+      <c r="AL82" t="inlineStr"/>
+      <c r="AM82" t="inlineStr"/>
+      <c r="AN82" t="inlineStr"/>
+      <c r="AO82" t="inlineStr"/>
+      <c r="AP82" t="inlineStr"/>
+      <c r="AQ82" t="inlineStr"/>
+      <c r="AR82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -7922,8 +8788,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=tSrz6r5LQik </t>
         </is>
       </c>
-      <c r="K83" t="inlineStr"/>
-      <c r="L83" t="inlineStr"/>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ebNPC] ebNPC1</t>
+        </is>
+      </c>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
@@ -7946,11 +8820,7 @@
         </is>
       </c>
       <c r="V83" t="inlineStr"/>
-      <c r="W83" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W83" t="inlineStr"/>
       <c r="X83" t="inlineStr"/>
       <c r="Y83" t="inlineStr"/>
       <c r="Z83" t="inlineStr"/>
@@ -7965,10 +8835,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH83" t="inlineStr"/>
-      <c r="AI83" t="inlineStr"/>
+      <c r="AH83" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI83" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ83" t="inlineStr"/>
       <c r="AK83" t="inlineStr"/>
+      <c r="AL83" t="inlineStr"/>
+      <c r="AM83" t="inlineStr"/>
+      <c r="AN83" t="inlineStr"/>
+      <c r="AO83" t="inlineStr"/>
+      <c r="AP83" t="inlineStr"/>
+      <c r="AQ83" t="inlineStr"/>
+      <c r="AR83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -8013,8 +8898,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=Uw6jWa_HHf4 </t>
         </is>
       </c>
-      <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=wwNPC] wwNPC1</t>
+        </is>
+      </c>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
@@ -8037,11 +8930,7 @@
         </is>
       </c>
       <c r="V84" t="inlineStr"/>
-      <c r="W84" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W84" t="inlineStr"/>
       <c r="X84" t="inlineStr"/>
       <c r="Y84" t="inlineStr"/>
       <c r="Z84" t="inlineStr"/>
@@ -8056,10 +8945,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH84" t="inlineStr"/>
-      <c r="AI84" t="inlineStr"/>
+      <c r="AH84" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI84" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ84" t="inlineStr"/>
       <c r="AK84" t="inlineStr"/>
+      <c r="AL84" t="inlineStr"/>
+      <c r="AM84" t="inlineStr"/>
+      <c r="AN84" t="inlineStr"/>
+      <c r="AO84" t="inlineStr"/>
+      <c r="AP84" t="inlineStr"/>
+      <c r="AQ84" t="inlineStr"/>
+      <c r="AR84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -8104,8 +9008,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=AzjyNRz2_Bo </t>
         </is>
       </c>
-      <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr"/>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=twNPC] twNPC1</t>
+        </is>
+      </c>
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
@@ -8128,11 +9040,7 @@
         </is>
       </c>
       <c r="V85" t="inlineStr"/>
-      <c r="W85" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W85" t="inlineStr"/>
       <c r="X85" t="inlineStr"/>
       <c r="Y85" t="inlineStr"/>
       <c r="Z85" t="inlineStr"/>
@@ -8147,10 +9055,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH85" t="inlineStr"/>
-      <c r="AI85" t="inlineStr"/>
+      <c r="AH85" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI85" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ85" t="inlineStr"/>
       <c r="AK85" t="inlineStr"/>
+      <c r="AL85" t="inlineStr"/>
+      <c r="AM85" t="inlineStr"/>
+      <c r="AN85" t="inlineStr"/>
+      <c r="AO85" t="inlineStr"/>
+      <c r="AP85" t="inlineStr"/>
+      <c r="AQ85" t="inlineStr"/>
+      <c r="AR85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -8195,8 +9118,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=VUsJlr1hezI </t>
         </is>
       </c>
-      <c r="K86" t="inlineStr"/>
-      <c r="L86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=twNPC] twNPC1</t>
+        </is>
+      </c>
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
@@ -8219,11 +9150,7 @@
         </is>
       </c>
       <c r="V86" t="inlineStr"/>
-      <c r="W86" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W86" t="inlineStr"/>
       <c r="X86" t="inlineStr"/>
       <c r="Y86" t="inlineStr"/>
       <c r="Z86" t="inlineStr"/>
@@ -8238,10 +9165,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH86" t="inlineStr"/>
-      <c r="AI86" t="inlineStr"/>
+      <c r="AH86" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI86" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ86" t="inlineStr"/>
       <c r="AK86" t="inlineStr"/>
+      <c r="AL86" t="inlineStr"/>
+      <c r="AM86" t="inlineStr"/>
+      <c r="AN86" t="inlineStr"/>
+      <c r="AO86" t="inlineStr"/>
+      <c r="AP86" t="inlineStr"/>
+      <c r="AQ86" t="inlineStr"/>
+      <c r="AR86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -8286,8 +9228,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=BPfR0OeyJpQ </t>
         </is>
       </c>
-      <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr"/>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=twNPC] twNPC1</t>
+        </is>
+      </c>
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr"/>
@@ -8310,11 +9260,7 @@
         </is>
       </c>
       <c r="V87" t="inlineStr"/>
-      <c r="W87" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W87" t="inlineStr"/>
       <c r="X87" t="inlineStr"/>
       <c r="Y87" t="inlineStr"/>
       <c r="Z87" t="inlineStr"/>
@@ -8329,10 +9275,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH87" t="inlineStr"/>
-      <c r="AI87" t="inlineStr"/>
+      <c r="AH87" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI87" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ87" t="inlineStr"/>
       <c r="AK87" t="inlineStr"/>
+      <c r="AL87" t="inlineStr"/>
+      <c r="AM87" t="inlineStr"/>
+      <c r="AN87" t="inlineStr"/>
+      <c r="AO87" t="inlineStr"/>
+      <c r="AP87" t="inlineStr"/>
+      <c r="AQ87" t="inlineStr"/>
+      <c r="AR87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -8377,8 +9338,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=e90k7FlJuJ0 </t>
         </is>
       </c>
-      <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr"/>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinendNPC] taliesinendNPC1</t>
+        </is>
+      </c>
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
@@ -8401,11 +9370,7 @@
         </is>
       </c>
       <c r="V88" t="inlineStr"/>
-      <c r="W88" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W88" t="inlineStr"/>
       <c r="X88" t="inlineStr"/>
       <c r="Y88" t="inlineStr"/>
       <c r="Z88" t="inlineStr"/>
@@ -8420,10 +9385,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH88" t="inlineStr"/>
-      <c r="AI88" t="inlineStr"/>
+      <c r="AH88" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI88" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ88" t="inlineStr"/>
       <c r="AK88" t="inlineStr"/>
+      <c r="AL88" t="inlineStr"/>
+      <c r="AM88" t="inlineStr"/>
+      <c r="AN88" t="inlineStr"/>
+      <c r="AO88" t="inlineStr"/>
+      <c r="AP88" t="inlineStr"/>
+      <c r="AQ88" t="inlineStr"/>
+      <c r="AR88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -8468,8 +9448,16 @@
           <t>https://www.youtube.com/watch_popup?v=xli79AKBnnY</t>
         </is>
       </c>
-      <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinendNPC] taliesinendNPC4</t>
+        </is>
+      </c>
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
@@ -8492,11 +9480,7 @@
         </is>
       </c>
       <c r="V89" t="inlineStr"/>
-      <c r="W89" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W89" t="inlineStr"/>
       <c r="X89" t="inlineStr"/>
       <c r="Y89" t="inlineStr"/>
       <c r="Z89" t="inlineStr"/>
@@ -8511,10 +9495,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH89" t="inlineStr"/>
-      <c r="AI89" t="inlineStr"/>
+      <c r="AH89" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI89" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ89" t="inlineStr"/>
       <c r="AK89" t="inlineStr"/>
+      <c r="AL89" t="inlineStr"/>
+      <c r="AM89" t="inlineStr"/>
+      <c r="AN89" t="inlineStr"/>
+      <c r="AO89" t="inlineStr"/>
+      <c r="AP89" t="inlineStr"/>
+      <c r="AQ89" t="inlineStr"/>
+      <c r="AR89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8559,8 +9558,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=beuv42HlpbA </t>
         </is>
       </c>
-      <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinendNPC] taliesinendNPC5</t>
+        </is>
+      </c>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
@@ -8583,11 +9590,7 @@
         </is>
       </c>
       <c r="V90" t="inlineStr"/>
-      <c r="W90" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W90" t="inlineStr"/>
       <c r="X90" t="inlineStr"/>
       <c r="Y90" t="inlineStr"/>
       <c r="Z90" t="inlineStr"/>
@@ -8602,10 +9605,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH90" t="inlineStr"/>
-      <c r="AI90" t="inlineStr"/>
+      <c r="AH90" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI90" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ90" t="inlineStr"/>
       <c r="AK90" t="inlineStr"/>
+      <c r="AL90" t="inlineStr"/>
+      <c r="AM90" t="inlineStr"/>
+      <c r="AN90" t="inlineStr"/>
+      <c r="AO90" t="inlineStr"/>
+      <c r="AP90" t="inlineStr"/>
+      <c r="AQ90" t="inlineStr"/>
+      <c r="AR90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -8650,8 +9668,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=2ey6ON0Ik7I </t>
         </is>
       </c>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinendNPC] taliesinendNPC6</t>
+        </is>
+      </c>
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
@@ -8674,11 +9700,7 @@
         </is>
       </c>
       <c r="V91" t="inlineStr"/>
-      <c r="W91" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W91" t="inlineStr"/>
       <c r="X91" t="inlineStr"/>
       <c r="Y91" t="inlineStr"/>
       <c r="Z91" t="inlineStr"/>
@@ -8693,10 +9715,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH91" t="inlineStr"/>
-      <c r="AI91" t="inlineStr"/>
+      <c r="AH91" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI91" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ91" t="inlineStr"/>
       <c r="AK91" t="inlineStr"/>
+      <c r="AL91" t="inlineStr"/>
+      <c r="AM91" t="inlineStr"/>
+      <c r="AN91" t="inlineStr"/>
+      <c r="AO91" t="inlineStr"/>
+      <c r="AP91" t="inlineStr"/>
+      <c r="AQ91" t="inlineStr"/>
+      <c r="AR91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -8741,8 +9778,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=0lECZey9-IA </t>
         </is>
       </c>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinendNPC] taliesinendNPC7</t>
+        </is>
+      </c>
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr"/>
@@ -8765,11 +9810,7 @@
         </is>
       </c>
       <c r="V92" t="inlineStr"/>
-      <c r="W92" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W92" t="inlineStr"/>
       <c r="X92" t="inlineStr"/>
       <c r="Y92" t="inlineStr"/>
       <c r="Z92" t="inlineStr"/>
@@ -8784,10 +9825,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH92" t="inlineStr"/>
-      <c r="AI92" t="inlineStr"/>
+      <c r="AH92" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI92" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ92" t="inlineStr"/>
       <c r="AK92" t="inlineStr"/>
+      <c r="AL92" t="inlineStr"/>
+      <c r="AM92" t="inlineStr"/>
+      <c r="AN92" t="inlineStr"/>
+      <c r="AO92" t="inlineStr"/>
+      <c r="AP92" t="inlineStr"/>
+      <c r="AQ92" t="inlineStr"/>
+      <c r="AR92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -8832,8 +9888,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=UqvHuyEwo1g </t>
         </is>
       </c>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinendNPC] taliesinendNPC8</t>
+        </is>
+      </c>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr"/>
@@ -8856,11 +9920,7 @@
         </is>
       </c>
       <c r="V93" t="inlineStr"/>
-      <c r="W93" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W93" t="inlineStr"/>
       <c r="X93" t="inlineStr"/>
       <c r="Y93" t="inlineStr"/>
       <c r="Z93" t="inlineStr"/>
@@ -8875,10 +9935,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH93" t="inlineStr"/>
-      <c r="AI93" t="inlineStr"/>
+      <c r="AH93" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI93" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ93" t="inlineStr"/>
       <c r="AK93" t="inlineStr"/>
+      <c r="AL93" t="inlineStr"/>
+      <c r="AM93" t="inlineStr"/>
+      <c r="AN93" t="inlineStr"/>
+      <c r="AO93" t="inlineStr"/>
+      <c r="AP93" t="inlineStr"/>
+      <c r="AQ93" t="inlineStr"/>
+      <c r="AR93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -8923,8 +9998,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=Yic4np31Flk </t>
         </is>
       </c>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=taliesinendNPC] taliesinendNPC9</t>
+        </is>
+      </c>
       <c r="M94" t="inlineStr"/>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
@@ -8947,11 +10030,7 @@
         </is>
       </c>
       <c r="V94" t="inlineStr"/>
-      <c r="W94" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W94" t="inlineStr"/>
       <c r="X94" t="inlineStr"/>
       <c r="Y94" t="inlineStr"/>
       <c r="Z94" t="inlineStr"/>
@@ -8966,10 +10045,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH94" t="inlineStr"/>
-      <c r="AI94" t="inlineStr"/>
+      <c r="AH94" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI94" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ94" t="inlineStr"/>
       <c r="AK94" t="inlineStr"/>
+      <c r="AL94" t="inlineStr"/>
+      <c r="AM94" t="inlineStr"/>
+      <c r="AN94" t="inlineStr"/>
+      <c r="AO94" t="inlineStr"/>
+      <c r="AP94" t="inlineStr"/>
+      <c r="AQ94" t="inlineStr"/>
+      <c r="AR94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -9014,8 +10108,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=DNPQ8xD2xi8 </t>
         </is>
       </c>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=dvlNPC] dvlNPC2</t>
+        </is>
+      </c>
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
@@ -9038,11 +10140,7 @@
         </is>
       </c>
       <c r="V95" t="inlineStr"/>
-      <c r="W95" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W95" t="inlineStr"/>
       <c r="X95" t="inlineStr"/>
       <c r="Y95" t="inlineStr"/>
       <c r="Z95" t="inlineStr"/>
@@ -9057,10 +10155,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH95" t="inlineStr"/>
-      <c r="AI95" t="inlineStr"/>
+      <c r="AH95" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI95" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ95" t="inlineStr"/>
       <c r="AK95" t="inlineStr"/>
+      <c r="AL95" t="inlineStr"/>
+      <c r="AM95" t="inlineStr"/>
+      <c r="AN95" t="inlineStr"/>
+      <c r="AO95" t="inlineStr"/>
+      <c r="AP95" t="inlineStr"/>
+      <c r="AQ95" t="inlineStr"/>
+      <c r="AR95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -9105,8 +10218,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=YbO8jQD8lXE </t>
         </is>
       </c>
-      <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr"/>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=dvlNPC] dvlNPC2</t>
+        </is>
+      </c>
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
@@ -9129,11 +10250,7 @@
         </is>
       </c>
       <c r="V96" t="inlineStr"/>
-      <c r="W96" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W96" t="inlineStr"/>
       <c r="X96" t="inlineStr"/>
       <c r="Y96" t="inlineStr"/>
       <c r="Z96" t="inlineStr"/>
@@ -9148,10 +10265,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH96" t="inlineStr"/>
-      <c r="AI96" t="inlineStr"/>
+      <c r="AH96" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI96" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ96" t="inlineStr"/>
       <c r="AK96" t="inlineStr"/>
+      <c r="AL96" t="inlineStr"/>
+      <c r="AM96" t="inlineStr"/>
+      <c r="AN96" t="inlineStr"/>
+      <c r="AO96" t="inlineStr"/>
+      <c r="AP96" t="inlineStr"/>
+      <c r="AQ96" t="inlineStr"/>
+      <c r="AR96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -9196,8 +10328,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=h1SvxuP9Q-k </t>
         </is>
       </c>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=dvlNPC] dvlNPC2</t>
+        </is>
+      </c>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
@@ -9220,11 +10360,7 @@
         </is>
       </c>
       <c r="V97" t="inlineStr"/>
-      <c r="W97" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W97" t="inlineStr"/>
       <c r="X97" t="inlineStr"/>
       <c r="Y97" t="inlineStr"/>
       <c r="Z97" t="inlineStr"/>
@@ -9239,10 +10375,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH97" t="inlineStr"/>
-      <c r="AI97" t="inlineStr"/>
+      <c r="AH97" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI97" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ97" t="inlineStr"/>
       <c r="AK97" t="inlineStr"/>
+      <c r="AL97" t="inlineStr"/>
+      <c r="AM97" t="inlineStr"/>
+      <c r="AN97" t="inlineStr"/>
+      <c r="AO97" t="inlineStr"/>
+      <c r="AP97" t="inlineStr"/>
+      <c r="AQ97" t="inlineStr"/>
+      <c r="AR97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -9287,8 +10438,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=4-RIrkS_2YY </t>
         </is>
       </c>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=dvlNPC] dvlNPC2</t>
+        </is>
+      </c>
       <c r="M98" t="inlineStr"/>
       <c r="N98" t="inlineStr"/>
       <c r="O98" t="inlineStr"/>
@@ -9311,11 +10470,7 @@
         </is>
       </c>
       <c r="V98" t="inlineStr"/>
-      <c r="W98" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W98" t="inlineStr"/>
       <c r="X98" t="inlineStr"/>
       <c r="Y98" t="inlineStr"/>
       <c r="Z98" t="inlineStr"/>
@@ -9330,10 +10485,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH98" t="inlineStr"/>
-      <c r="AI98" t="inlineStr"/>
+      <c r="AH98" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI98" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ98" t="inlineStr"/>
       <c r="AK98" t="inlineStr"/>
+      <c r="AL98" t="inlineStr"/>
+      <c r="AM98" t="inlineStr"/>
+      <c r="AN98" t="inlineStr"/>
+      <c r="AO98" t="inlineStr"/>
+      <c r="AP98" t="inlineStr"/>
+      <c r="AQ98" t="inlineStr"/>
+      <c r="AR98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -9378,8 +10548,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=Mak69hjejw0 </t>
         </is>
       </c>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr"/>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=dvlNPC] dvlNPC2</t>
+        </is>
+      </c>
       <c r="M99" t="inlineStr"/>
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr"/>
@@ -9402,11 +10580,7 @@
         </is>
       </c>
       <c r="V99" t="inlineStr"/>
-      <c r="W99" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W99" t="inlineStr"/>
       <c r="X99" t="inlineStr"/>
       <c r="Y99" t="inlineStr"/>
       <c r="Z99" t="inlineStr"/>
@@ -9421,10 +10595,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH99" t="inlineStr"/>
-      <c r="AI99" t="inlineStr"/>
+      <c r="AH99" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI99" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ99" t="inlineStr"/>
       <c r="AK99" t="inlineStr"/>
+      <c r="AL99" t="inlineStr"/>
+      <c r="AM99" t="inlineStr"/>
+      <c r="AN99" t="inlineStr"/>
+      <c r="AO99" t="inlineStr"/>
+      <c r="AP99" t="inlineStr"/>
+      <c r="AQ99" t="inlineStr"/>
+      <c r="AR99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -9469,8 +10658,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=K2pzYWqkwm0 </t>
         </is>
       </c>
-      <c r="K100" t="inlineStr"/>
-      <c r="L100" t="inlineStr"/>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=mmbNPC] mmbNPC2</t>
+        </is>
+      </c>
       <c r="M100" t="inlineStr"/>
       <c r="N100" t="inlineStr"/>
       <c r="O100" t="inlineStr"/>
@@ -9493,11 +10690,7 @@
         </is>
       </c>
       <c r="V100" t="inlineStr"/>
-      <c r="W100" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W100" t="inlineStr"/>
       <c r="X100" t="inlineStr"/>
       <c r="Y100" t="inlineStr"/>
       <c r="Z100" t="inlineStr"/>
@@ -9512,10 +10705,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH100" t="inlineStr"/>
-      <c r="AI100" t="inlineStr"/>
+      <c r="AH100" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI100" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ100" t="inlineStr"/>
       <c r="AK100" t="inlineStr"/>
+      <c r="AL100" t="inlineStr"/>
+      <c r="AM100" t="inlineStr"/>
+      <c r="AN100" t="inlineStr"/>
+      <c r="AO100" t="inlineStr"/>
+      <c r="AP100" t="inlineStr"/>
+      <c r="AQ100" t="inlineStr"/>
+      <c r="AR100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -9560,8 +10768,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=WWBpn9vPZwE </t>
         </is>
       </c>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=mmbNPC] mmbNPC2</t>
+        </is>
+      </c>
       <c r="M101" t="inlineStr"/>
       <c r="N101" t="inlineStr"/>
       <c r="O101" t="inlineStr"/>
@@ -9584,11 +10800,7 @@
         </is>
       </c>
       <c r="V101" t="inlineStr"/>
-      <c r="W101" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W101" t="inlineStr"/>
       <c r="X101" t="inlineStr"/>
       <c r="Y101" t="inlineStr"/>
       <c r="Z101" t="inlineStr"/>
@@ -9603,10 +10815,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH101" t="inlineStr"/>
-      <c r="AI101" t="inlineStr"/>
+      <c r="AH101" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI101" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ101" t="inlineStr"/>
       <c r="AK101" t="inlineStr"/>
+      <c r="AL101" t="inlineStr"/>
+      <c r="AM101" t="inlineStr"/>
+      <c r="AN101" t="inlineStr"/>
+      <c r="AO101" t="inlineStr"/>
+      <c r="AP101" t="inlineStr"/>
+      <c r="AQ101" t="inlineStr"/>
+      <c r="AR101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -9651,8 +10878,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=6lZ7qT-g5dM  </t>
         </is>
       </c>
-      <c r="K102" t="inlineStr"/>
-      <c r="L102" t="inlineStr"/>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=mmbNPC] mmbNPC3</t>
+        </is>
+      </c>
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="inlineStr"/>
       <c r="O102" t="inlineStr"/>
@@ -9675,11 +10910,7 @@
         </is>
       </c>
       <c r="V102" t="inlineStr"/>
-      <c r="W102" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W102" t="inlineStr"/>
       <c r="X102" t="inlineStr"/>
       <c r="Y102" t="inlineStr"/>
       <c r="Z102" t="inlineStr"/>
@@ -9694,10 +10925,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH102" t="inlineStr"/>
-      <c r="AI102" t="inlineStr"/>
+      <c r="AH102" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI102" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ102" t="inlineStr"/>
       <c r="AK102" t="inlineStr"/>
+      <c r="AL102" t="inlineStr"/>
+      <c r="AM102" t="inlineStr"/>
+      <c r="AN102" t="inlineStr"/>
+      <c r="AO102" t="inlineStr"/>
+      <c r="AP102" t="inlineStr"/>
+      <c r="AQ102" t="inlineStr"/>
+      <c r="AR102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -9742,8 +10988,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=g9sB8U-V32c </t>
         </is>
       </c>
-      <c r="K103" t="inlineStr"/>
-      <c r="L103" t="inlineStr"/>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=sgNPC] sgNPC2</t>
+        </is>
+      </c>
       <c r="M103" t="inlineStr"/>
       <c r="N103" t="inlineStr"/>
       <c r="O103" t="inlineStr"/>
@@ -9766,11 +11020,7 @@
         </is>
       </c>
       <c r="V103" t="inlineStr"/>
-      <c r="W103" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W103" t="inlineStr"/>
       <c r="X103" t="inlineStr"/>
       <c r="Y103" t="inlineStr"/>
       <c r="Z103" t="inlineStr"/>
@@ -9785,10 +11035,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH103" t="inlineStr"/>
-      <c r="AI103" t="inlineStr"/>
+      <c r="AH103" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI103" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ103" t="inlineStr"/>
       <c r="AK103" t="inlineStr"/>
+      <c r="AL103" t="inlineStr"/>
+      <c r="AM103" t="inlineStr"/>
+      <c r="AN103" t="inlineStr"/>
+      <c r="AO103" t="inlineStr"/>
+      <c r="AP103" t="inlineStr"/>
+      <c r="AQ103" t="inlineStr"/>
+      <c r="AR103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -9833,8 +11098,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=8ebN-3yfATs </t>
         </is>
       </c>
-      <c r="K104" t="inlineStr"/>
-      <c r="L104" t="inlineStr"/>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ffqNPC] ffqNPC2</t>
+        </is>
+      </c>
       <c r="M104" t="inlineStr"/>
       <c r="N104" t="inlineStr"/>
       <c r="O104" t="inlineStr"/>
@@ -9857,11 +11130,7 @@
         </is>
       </c>
       <c r="V104" t="inlineStr"/>
-      <c r="W104" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W104" t="inlineStr"/>
       <c r="X104" t="inlineStr"/>
       <c r="Y104" t="inlineStr"/>
       <c r="Z104" t="inlineStr"/>
@@ -9876,10 +11145,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH104" t="inlineStr"/>
-      <c r="AI104" t="inlineStr"/>
+      <c r="AH104" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI104" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ104" t="inlineStr"/>
       <c r="AK104" t="inlineStr"/>
+      <c r="AL104" t="inlineStr"/>
+      <c r="AM104" t="inlineStr"/>
+      <c r="AN104" t="inlineStr"/>
+      <c r="AO104" t="inlineStr"/>
+      <c r="AP104" t="inlineStr"/>
+      <c r="AQ104" t="inlineStr"/>
+      <c r="AR104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -9924,8 +11208,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=sjYbBZeyNBU </t>
         </is>
       </c>
-      <c r="K105" t="inlineStr"/>
-      <c r="L105" t="inlineStr"/>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ffqNPC] ffqNPC2</t>
+        </is>
+      </c>
       <c r="M105" t="inlineStr"/>
       <c r="N105" t="inlineStr"/>
       <c r="O105" t="inlineStr"/>
@@ -9948,11 +11240,7 @@
         </is>
       </c>
       <c r="V105" t="inlineStr"/>
-      <c r="W105" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W105" t="inlineStr"/>
       <c r="X105" t="inlineStr"/>
       <c r="Y105" t="inlineStr"/>
       <c r="Z105" t="inlineStr"/>
@@ -9967,10 +11255,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH105" t="inlineStr"/>
-      <c r="AI105" t="inlineStr"/>
+      <c r="AH105" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI105" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ105" t="inlineStr"/>
       <c r="AK105" t="inlineStr"/>
+      <c r="AL105" t="inlineStr"/>
+      <c r="AM105" t="inlineStr"/>
+      <c r="AN105" t="inlineStr"/>
+      <c r="AO105" t="inlineStr"/>
+      <c r="AP105" t="inlineStr"/>
+      <c r="AQ105" t="inlineStr"/>
+      <c r="AR105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -10015,8 +11318,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=NwLimldTi9U </t>
         </is>
       </c>
-      <c r="K106" t="inlineStr"/>
-      <c r="L106" t="inlineStr"/>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=flfNPC] flfNPC1</t>
+        </is>
+      </c>
       <c r="M106" t="inlineStr"/>
       <c r="N106" t="inlineStr"/>
       <c r="O106" t="inlineStr"/>
@@ -10039,11 +11350,7 @@
         </is>
       </c>
       <c r="V106" t="inlineStr"/>
-      <c r="W106" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W106" t="inlineStr"/>
       <c r="X106" t="inlineStr"/>
       <c r="Y106" t="inlineStr"/>
       <c r="Z106" t="inlineStr"/>
@@ -10058,10 +11365,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH106" t="inlineStr"/>
-      <c r="AI106" t="inlineStr"/>
+      <c r="AH106" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI106" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ106" t="inlineStr"/>
       <c r="AK106" t="inlineStr"/>
+      <c r="AL106" t="inlineStr"/>
+      <c r="AM106" t="inlineStr"/>
+      <c r="AN106" t="inlineStr"/>
+      <c r="AO106" t="inlineStr"/>
+      <c r="AP106" t="inlineStr"/>
+      <c r="AQ106" t="inlineStr"/>
+      <c r="AR106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -10106,8 +11428,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=y6rCTGg7Tn0 </t>
         </is>
       </c>
-      <c r="K107" t="inlineStr"/>
-      <c r="L107" t="inlineStr"/>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=flfNPC] flfNPC1</t>
+        </is>
+      </c>
       <c r="M107" t="inlineStr"/>
       <c r="N107" t="inlineStr"/>
       <c r="O107" t="inlineStr"/>
@@ -10130,11 +11460,7 @@
         </is>
       </c>
       <c r="V107" t="inlineStr"/>
-      <c r="W107" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W107" t="inlineStr"/>
       <c r="X107" t="inlineStr"/>
       <c r="Y107" t="inlineStr"/>
       <c r="Z107" t="inlineStr"/>
@@ -10149,10 +11475,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH107" t="inlineStr"/>
-      <c r="AI107" t="inlineStr"/>
+      <c r="AH107" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI107" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ107" t="inlineStr"/>
       <c r="AK107" t="inlineStr"/>
+      <c r="AL107" t="inlineStr"/>
+      <c r="AM107" t="inlineStr"/>
+      <c r="AN107" t="inlineStr"/>
+      <c r="AO107" t="inlineStr"/>
+      <c r="AP107" t="inlineStr"/>
+      <c r="AQ107" t="inlineStr"/>
+      <c r="AR107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -10197,8 +11538,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=ghuiaCTgu1w </t>
         </is>
       </c>
-      <c r="K108" t="inlineStr"/>
-      <c r="L108" t="inlineStr"/>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=flfNPC] flfNPC1</t>
+        </is>
+      </c>
       <c r="M108" t="inlineStr"/>
       <c r="N108" t="inlineStr"/>
       <c r="O108" t="inlineStr"/>
@@ -10221,11 +11570,7 @@
         </is>
       </c>
       <c r="V108" t="inlineStr"/>
-      <c r="W108" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W108" t="inlineStr"/>
       <c r="X108" t="inlineStr"/>
       <c r="Y108" t="inlineStr"/>
       <c r="Z108" t="inlineStr"/>
@@ -10240,10 +11585,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH108" t="inlineStr"/>
-      <c r="AI108" t="inlineStr"/>
+      <c r="AH108" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI108" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ108" t="inlineStr"/>
       <c r="AK108" t="inlineStr"/>
+      <c r="AL108" t="inlineStr"/>
+      <c r="AM108" t="inlineStr"/>
+      <c r="AN108" t="inlineStr"/>
+      <c r="AO108" t="inlineStr"/>
+      <c r="AP108" t="inlineStr"/>
+      <c r="AQ108" t="inlineStr"/>
+      <c r="AR108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -10288,8 +11648,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=fgIZt2-Nx_w </t>
         </is>
       </c>
-      <c r="K109" t="inlineStr"/>
-      <c r="L109" t="inlineStr"/>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ctcNPC] ctcNPC1</t>
+        </is>
+      </c>
       <c r="M109" t="inlineStr"/>
       <c r="N109" t="inlineStr"/>
       <c r="O109" t="inlineStr"/>
@@ -10312,11 +11680,7 @@
         </is>
       </c>
       <c r="V109" t="inlineStr"/>
-      <c r="W109" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W109" t="inlineStr"/>
       <c r="X109" t="inlineStr"/>
       <c r="Y109" t="inlineStr"/>
       <c r="Z109" t="inlineStr"/>
@@ -10331,10 +11695,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH109" t="inlineStr"/>
-      <c r="AI109" t="inlineStr"/>
+      <c r="AH109" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI109" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ109" t="inlineStr"/>
       <c r="AK109" t="inlineStr"/>
+      <c r="AL109" t="inlineStr"/>
+      <c r="AM109" t="inlineStr"/>
+      <c r="AN109" t="inlineStr"/>
+      <c r="AO109" t="inlineStr"/>
+      <c r="AP109" t="inlineStr"/>
+      <c r="AQ109" t="inlineStr"/>
+      <c r="AR109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -10379,8 +11758,16 @@
           <t xml:space="preserve">https://www.youtube.com/watch_popup?v=OCILZG5lh_A </t>
         </is>
       </c>
-      <c r="K110" t="inlineStr"/>
-      <c r="L110" t="inlineStr"/>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>dialogue open @e[tag=ctcNPC] ctcNPC1</t>
+        </is>
+      </c>
       <c r="M110" t="inlineStr"/>
       <c r="N110" t="inlineStr"/>
       <c r="O110" t="inlineStr"/>
@@ -10403,11 +11790,7 @@
         </is>
       </c>
       <c r="V110" t="inlineStr"/>
-      <c r="W110" t="inlineStr">
-        <is>
-          <t>Cymraeg</t>
-        </is>
-      </c>
+      <c r="W110" t="inlineStr"/>
       <c r="X110" t="inlineStr"/>
       <c r="Y110" t="inlineStr"/>
       <c r="Z110" t="inlineStr"/>
@@ -10422,10 +11805,25 @@
           <t>Cymraeg</t>
         </is>
       </c>
-      <c r="AH110" t="inlineStr"/>
-      <c r="AI110" t="inlineStr"/>
+      <c r="AH110" t="inlineStr">
+        <is>
+          <t>Yn ôl</t>
+        </is>
+      </c>
+      <c r="AI110" t="inlineStr">
+        <is>
+          <t>Cymraeg</t>
+        </is>
+      </c>
       <c r="AJ110" t="inlineStr"/>
       <c r="AK110" t="inlineStr"/>
+      <c r="AL110" t="inlineStr"/>
+      <c r="AM110" t="inlineStr"/>
+      <c r="AN110" t="inlineStr"/>
+      <c r="AO110" t="inlineStr"/>
+      <c r="AP110" t="inlineStr"/>
+      <c r="AQ110" t="inlineStr"/>
+      <c r="AR110" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>